<commit_message>
Update pipeline code, configs, and data assets
</commit_message>
<xml_diff>
--- a/00_selection/vendor_map.xlsx
+++ b/00_selection/vendor_map.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29426"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selsherb\Documents\VENDRIX\00_selection\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\selsherb\Documents\Prototype\00_selection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB2D95DB-9C46-4ACC-92DD-51ADF1D9512F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C674F8B-F6F5-42EE-AD26-8F168EA64B67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -390,7 +390,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>